<commit_message>
agregado nuevo escenario y automatización para iniciar sesión
</commit_message>
<xml_diff>
--- a/parametros/Datos.xlsx
+++ b/parametros/Datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semillero QA\TempletePOM\parametros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B263D45B-A78B-4197-8F52-2337CBBE124D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BAFAA7-567A-410E-BA4C-2E17C3AF83B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,10 +106,10 @@
     <t>Clave</t>
   </si>
   <si>
-    <t>gutierrez.012900@gmail.com</t>
-  </si>
-  <si>
-    <t>123456ABC*</t>
+    <t>paangudi3@gmail.com</t>
+  </si>
+  <si>
+    <t>12345ABC*</t>
   </si>
 </sst>
 </file>
@@ -596,7 +596,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,7 +615,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -623,7 +623,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{0660574E-77E3-4FF5-8CCE-2363ADACBE83}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>